<commit_message>
refactor excel and dao
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/template/i18n_properties.xlsx
+++ b/src/main/webapp/resources/template/i18n_properties.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="simulator" sheetId="1" r:id="rId1"/>
-    <sheet name="master" sheetId="2" r:id="rId2"/>
-    <sheet name="pog" sheetId="3" r:id="rId3"/>
+    <sheet name="common" sheetId="1" r:id="rId1"/>
+    <sheet name="simulator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>zh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,10 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上传</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,6 +102,26 @@
   </si>
   <si>
     <t>Télécharger</t>
+  </si>
+  <si>
+    <t>on create 4 versions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只能存储4个版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peut stocker 4 versions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version.overflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -546,7 +561,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -568,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -582,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -596,7 +611,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -610,7 +625,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -624,7 +639,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -632,13 +647,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -650,29 +665,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="4" max="4" width="27.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add dictionaray and ui plugins
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/template/i18n_properties.xlsx
+++ b/src/main/webapp/resources/template/i18n_properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>zh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,7 +120,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上传1</t>
+    <t>store_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>store_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Le nom de magasin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Le Code de magasin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exporter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -558,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -647,13 +695,27 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -665,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -707,6 +769,34 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
export enhance,export do my oneself
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/template/i18n_properties.xlsx
+++ b/src/main/webapp/resources/template/i18n_properties.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="common" sheetId="1" r:id="rId1"/>
     <sheet name="simulator" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>zh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -169,14 +169,42 @@
   </si>
   <si>
     <t>导出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status.active</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLOSED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开启</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status.closed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,74 +271,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -320,14 +280,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -394,7 +354,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -429,7 +388,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -605,14 +563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
@@ -620,7 +578,7 @@
     <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -634,7 +592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="27">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -648,7 +606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="27">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -662,7 +620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="27">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -676,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="27">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -690,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="27">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -704,7 +662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="27">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -716,6 +674,34 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -726,14 +712,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="21.625" customWidth="1"/>
     <col min="2" max="2" width="23.125" customWidth="1"/>
@@ -741,7 +727,7 @@
     <col min="4" max="4" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -755,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -769,7 +755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -783,7 +769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>28</v>
       </c>

</xml_diff>